<commit_message>
Instructions, python script and error handling
- Added the instructions and executable python script

- Added an error handling to write an excel file with an error message instead if the optimisation was not successfully terminated

- Updated the excel_sharpe python script
</commit_message>
<xml_diff>
--- a/Optimise_Sharpe/stock_input_file.xlsx
+++ b/Optimise_Sharpe/stock_input_file.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mark/Documents/Coding practice/Python_Finance/Optimise_Sharpe/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F814166-04C4-5B49-AC1D-20BC8272116E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD13FC58-2750-024E-BF96-91AEEC6658BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="680" yWindow="740" windowWidth="28040" windowHeight="16960" xr2:uid="{756C99D0-0F0D-0E4B-B65F-304C87498D43}"/>
   </bookViews>
@@ -198,7 +198,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
@@ -236,16 +236,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="17">
     <dxf>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -291,6 +287,9 @@
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
       <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -329,47 +328,47 @@
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{E4E1FDB9-AF36-3449-99B1-6DD784142C5F}" name="Stock Ticker" dataDxfId="14"/>
     <tableColumn id="2" xr3:uid="{AD7045D3-5A3E-4540-98B1-ADEEA1A9E625}" name="Amount Invested" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{1F6EE3F0-9A5E-E74B-83E4-FC22B7F08B4F}" name="Max Portfolio Weight" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{1F6EE3F0-9A5E-E74B-83E4-FC22B7F08B4F}" name="Max Portfolio Weight" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B6D7C18B-6731-3E40-85F7-3261E29451C8}" name="Table2" displayName="Table2" ref="A1:A2" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B6D7C18B-6731-3E40-85F7-3261E29451C8}" name="Table2" displayName="Table2" ref="A1:A2" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="A1:A2" xr:uid="{B6D7C18B-6731-3E40-85F7-3261E29451C8}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{673F99A4-2A3A-D342-9B69-CAE54EBCE8AA}" name="Annual Risk Free Rate" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{673F99A4-2A3A-D342-9B69-CAE54EBCE8AA}" name="Annual Risk Free Rate" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{DE643D75-5A06-1D4B-9F12-76170568C61F}" name="Table4" displayName="Table4" ref="B1:B2" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{DE643D75-5A06-1D4B-9F12-76170568C61F}" name="Table4" displayName="Table4" ref="B1:B2" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <autoFilter ref="B1:B2" xr:uid="{DE643D75-5A06-1D4B-9F12-76170568C61F}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{FD6CFC6B-AE91-104C-BF41-2FB88AB655AF}" name="Time Interval" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{FD6CFC6B-AE91-104C-BF41-2FB88AB655AF}" name="Time Interval" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{746FEE24-3AC8-F54A-B66E-326D504A5A4D}" name="Table5" displayName="Table5" ref="C1:C2" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{746FEE24-3AC8-F54A-B66E-326D504A5A4D}" name="Table5" displayName="Table5" ref="C1:C2" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <autoFilter ref="C1:C2" xr:uid="{746FEE24-3AC8-F54A-B66E-326D504A5A4D}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{68CB6ED0-AB54-FB44-9379-5355FF31D79F}" name="Start Date" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{68CB6ED0-AB54-FB44-9379-5355FF31D79F}" name="Start Date" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{70BD5DC6-07D1-334F-9425-4D4C92D90C70}" name="Table6" displayName="Table6" ref="D1:D2" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{70BD5DC6-07D1-334F-9425-4D4C92D90C70}" name="Table6" displayName="Table6" ref="D1:D2" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
   <autoFilter ref="D1:D2" xr:uid="{70BD5DC6-07D1-334F-9425-4D4C92D90C70}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{B9AA6F25-A7C2-E146-95F3-F25715C7A69D}" name="End Date" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{B9AA6F25-A7C2-E146-95F3-F25715C7A69D}" name="End Date" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -695,7 +694,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -712,7 +711,7 @@
       <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>